<commit_message>
modifie le repo Liste+Bilan Contrat en utilisant le noveau contrat notes et jury
</commit_message>
<xml_diff>
--- a/Liste+Bilan contrat/ListeContrats+Bilan/bilanContrat.xlsx
+++ b/Liste+Bilan contrat/ListeContrats+Bilan/bilanContrat.xlsx
@@ -107,12 +107,12 @@
     <t xml:space="preserve">EC-STP03-ACSA</t>
   </si>
   <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">Chimie 3</t>
   </si>
   <si>
@@ -164,6 +164,15 @@
     <t xml:space="preserve">EC-STP03-MECA</t>
   </si>
   <si>
+    <t xml:space="preserve">Stage (UE-STP03-STAG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC-STP03-STAG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orientation et Transition (UE-STP03-ORT)</t>
   </si>
   <si>
@@ -216,15 +225,6 @@
   </si>
   <si>
     <t xml:space="preserve">EC-STP03-LV2EC-STP03-FLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage (UE-STP03-STAG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EC-STP03-STAG</t>
   </si>
   <si>
     <t xml:space="preserve">Sciences expérimentales (UE-STP04-SE)</t>
@@ -767,46 +767,46 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
         <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T2" t="s">
         <v>31</v>
@@ -815,13 +815,13 @@
         <v>31</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W2" t="s">
         <v>31</v>
       </c>
       <c r="X2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y2" t="s">
         <v>32</v>
@@ -830,15 +830,15 @@
         <v>31</v>
       </c>
       <c r="AA2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -847,28 +847,28 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -877,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -886,22 +886,22 @@
         <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S3" t="s">
         <v>31</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W3" t="s">
         <v>31</v>
@@ -910,21 +910,21 @@
         <v>32</v>
       </c>
       <c r="Y3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z3" t="s">
         <v>31</v>
       </c>
       <c r="AA3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -933,19 +933,19 @@
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
         <v>31</v>
@@ -954,22 +954,22 @@
         <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
         <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" t="s">
         <v>31</v>
@@ -990,10 +990,10 @@
         <v>31</v>
       </c>
       <c r="W4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y4" t="s">
         <v>32</v>
@@ -1002,7 +1002,7 @@
         <v>31</v>
       </c>
       <c r="AA4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB4" t="s">
         <v>32</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -1022,7 +1022,7 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
@@ -1034,16 +1034,16 @@
         <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -1058,19 +1058,19 @@
         <v>31</v>
       </c>
       <c r="Q5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T5" t="s">
         <v>31</v>
       </c>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V5" t="s">
         <v>32</v>
@@ -1082,13 +1082,13 @@
         <v>32</v>
       </c>
       <c r="Y5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z5" t="s">
         <v>31</v>
       </c>
       <c r="AA5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB5" t="s">
         <v>32</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1120,40 +1120,40 @@
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S6" t="s">
         <v>31</v>
       </c>
       <c r="T6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U6" t="s">
         <v>31</v>
@@ -1162,19 +1162,19 @@
         <v>31</v>
       </c>
       <c r="W6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z6" t="s">
         <v>31</v>
       </c>
       <c r="AA6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB6" t="s">
         <v>31</v>
@@ -1200,25 +1200,25 @@
         <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
         <v>32</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
         <v>31</v>
@@ -1236,39 +1236,39 @@
         <v>31</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V7" t="s">
         <v>31</v>
       </c>
       <c r="W7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X7" t="s">
         <v>31</v>
       </c>
       <c r="Y7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -1280,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
@@ -1289,10 +1289,10 @@
         <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
         <v>32</v>
@@ -1301,13 +1301,13 @@
         <v>31</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M8" t="s">
         <v>31</v>
       </c>
       <c r="N8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O8" t="s">
         <v>31</v>
@@ -1322,31 +1322,31 @@
         <v>31</v>
       </c>
       <c r="S8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W8" t="s">
         <v>31</v>
       </c>
       <c r="X8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y8" t="s">
         <v>31</v>
       </c>
       <c r="Z8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB8" t="s">
         <v>31</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>46</v>
@@ -1363,40 +1363,40 @@
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N9" t="s">
         <v>31</v>
       </c>
       <c r="O9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P9" t="s">
         <v>31</v>
@@ -1405,22 +1405,22 @@
         <v>31</v>
       </c>
       <c r="R9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S9" t="s">
         <v>32</v>
       </c>
       <c r="T9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V9" t="s">
         <v>31</v>
       </c>
       <c r="W9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X9" t="s">
         <v>31</v>
@@ -1429,10 +1429,10 @@
         <v>31</v>
       </c>
       <c r="Z9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB9" t="s">
         <v>31</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -1452,64 +1452,64 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J10" t="s">
         <v>31</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N10" t="s">
         <v>32</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P10" t="s">
         <v>32</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T10" t="s">
         <v>32</v>
       </c>
       <c r="U10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W10" t="s">
         <v>31</v>
       </c>
       <c r="X10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y10" t="s">
         <v>31</v>
@@ -1521,7 +1521,7 @@
         <v>31</v>
       </c>
       <c r="AB10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1544,10 +1544,10 @@
         <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -1562,49 +1562,49 @@
         <v>31</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N11" t="s">
         <v>32</v>
       </c>
       <c r="O11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q11" t="s">
         <v>32</v>
       </c>
       <c r="R11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U11" t="s">
         <v>32</v>
       </c>
       <c r="V11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W11" t="s">
         <v>32</v>
       </c>
       <c r="X11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y11" t="s">
         <v>32</v>
       </c>
       <c r="Z11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB11" t="s">
         <v>32</v>
@@ -1612,19 +1612,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1639,78 +1639,78 @@
         <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K12" t="s">
         <v>31</v>
       </c>
       <c r="L12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
@@ -1725,72 +1725,72 @@
         <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K13" t="s">
         <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
         <v>31</v>
@@ -1808,61 +1808,61 @@
         <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" t="s">
         <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
         <v>32</v>
       </c>
       <c r="M14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" t="s">
         <v>31</v>
       </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q14" t="s">
         <v>31</v>
       </c>
       <c r="R14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U14" t="s">
         <v>31</v>
       </c>
       <c r="V14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W14" t="s">
         <v>31</v>
       </c>
       <c r="X14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y14" t="s">
         <v>31</v>
       </c>
       <c r="Z14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB14" t="s">
         <v>31</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
@@ -1879,10 +1879,10 @@
         <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
@@ -1897,324 +1897,324 @@
         <v>31</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K15" t="s">
         <v>31</v>
       </c>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" t="s">
         <v>31</v>
       </c>
       <c r="J16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16" t="s">
         <v>31</v>
       </c>
       <c r="N16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R16" t="s">
         <v>31</v>
       </c>
       <c r="S16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R17" t="s">
         <v>31</v>
       </c>
       <c r="S17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V17" t="s">
         <v>31</v>
       </c>
       <c r="W17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA17" t="s">
         <v>31</v>
       </c>
       <c r="AB17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
         <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I18" t="s">
         <v>31</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>69</v>
@@ -2223,79 +2223,79 @@
         <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
         <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" t="s">
         <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K19" t="s">
         <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V19" t="s">
         <v>31</v>
       </c>
       <c r="W19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA19" t="s">
         <v>31</v>
       </c>
       <c r="AB19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20">
@@ -2309,19 +2309,19 @@
         <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
         <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
         <v>31</v>
@@ -2333,37 +2333,37 @@
         <v>32</v>
       </c>
       <c r="L20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R20" t="s">
         <v>31</v>
       </c>
       <c r="S20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U20" t="s">
         <v>32</v>
       </c>
       <c r="V20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W20" t="s">
         <v>32</v>
@@ -2372,21 +2372,21 @@
         <v>31</v>
       </c>
       <c r="Y20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -2398,22 +2398,22 @@
         <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" t="s">
         <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K21" t="s">
         <v>31</v>
@@ -2428,19 +2428,19 @@
         <v>31</v>
       </c>
       <c r="O21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q21" t="s">
         <v>31</v>
       </c>
       <c r="R21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T21" t="s">
         <v>31</v>
@@ -2449,30 +2449,30 @@
         <v>32</v>
       </c>
       <c r="V21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W21" t="s">
         <v>32</v>
       </c>
       <c r="X21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
@@ -2481,7 +2481,7 @@
         <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
         <v>32</v>
@@ -2490,13 +2490,13 @@
         <v>32</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J22" t="s">
         <v>31</v>
@@ -2508,13 +2508,13 @@
         <v>31</v>
       </c>
       <c r="M22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N22" t="s">
         <v>32</v>
       </c>
       <c r="O22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P22" t="s">
         <v>31</v>
@@ -2523,10 +2523,10 @@
         <v>31</v>
       </c>
       <c r="R22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T22" t="s">
         <v>31</v>
@@ -2553,12 +2553,12 @@
         <v>32</v>
       </c>
       <c r="AB22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
@@ -2573,28 +2573,28 @@
         <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N23" t="s">
         <v>31</v>
@@ -2603,22 +2603,22 @@
         <v>31</v>
       </c>
       <c r="P23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V23" t="s">
         <v>32</v>
@@ -2630,21 +2630,21 @@
         <v>31</v>
       </c>
       <c r="Y23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>80</v>
@@ -2653,7 +2653,7 @@
         <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>31</v>
@@ -2668,69 +2668,69 @@
         <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
         <v>31</v>
       </c>
       <c r="K24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L24" t="s">
         <v>31</v>
       </c>
       <c r="M24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N24" t="s">
         <v>32</v>
       </c>
       <c r="O24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P24" t="s">
         <v>31</v>
       </c>
       <c r="Q24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R24" t="s">
         <v>32</v>
       </c>
       <c r="S24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V24" t="s">
         <v>32</v>
       </c>
       <c r="W24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z24" t="s">
         <v>31</v>
       </c>
       <c r="AA24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
@@ -2745,7 +2745,7 @@
         <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25" t="s">
         <v>31</v>
@@ -2757,16 +2757,16 @@
         <v>31</v>
       </c>
       <c r="J25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N25" t="s">
         <v>31</v>
@@ -2775,7 +2775,7 @@
         <v>31</v>
       </c>
       <c r="P25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q25" t="s">
         <v>31</v>
@@ -2784,19 +2784,19 @@
         <v>32</v>
       </c>
       <c r="S25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T25" t="s">
         <v>31</v>
       </c>
       <c r="U25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X25" t="s">
         <v>31</v>
@@ -2808,7 +2808,7 @@
         <v>31</v>
       </c>
       <c r="AA25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB25" t="s">
         <v>32</v>
@@ -2834,13 +2834,13 @@
         <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J26" t="s">
         <v>32</v>
@@ -2849,28 +2849,28 @@
         <v>31</v>
       </c>
       <c r="L26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N26" t="s">
         <v>32</v>
       </c>
       <c r="O26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T26" t="s">
         <v>31</v>
@@ -2882,7 +2882,7 @@
         <v>31</v>
       </c>
       <c r="W26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X26" t="s">
         <v>32</v>
@@ -2891,7 +2891,7 @@
         <v>31</v>
       </c>
       <c r="Z26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA26" t="s">
         <v>31</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>87</v>
@@ -2923,28 +2923,28 @@
         <v>31</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K27" t="s">
         <v>32</v>
       </c>
       <c r="L27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M27" t="s">
         <v>31</v>
       </c>
       <c r="N27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
@@ -2956,10 +2956,10 @@
         <v>31</v>
       </c>
       <c r="S27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U27" t="s">
         <v>31</v>
@@ -2974,21 +2974,21 @@
         <v>31</v>
       </c>
       <c r="Y27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
@@ -3000,7 +3000,7 @@
         <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
         <v>31</v>
@@ -3009,7 +3009,7 @@
         <v>31</v>
       </c>
       <c r="H28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I28" t="s">
         <v>31</v>
@@ -3024,13 +3024,13 @@
         <v>32</v>
       </c>
       <c r="M28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P28" t="s">
         <v>32</v>
@@ -3042,25 +3042,25 @@
         <v>31</v>
       </c>
       <c r="S28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U28" t="s">
         <v>31</v>
       </c>
       <c r="V28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X28" t="s">
         <v>32</v>
       </c>
       <c r="Y28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z28" t="s">
         <v>31</v>
@@ -3083,84 +3083,84 @@
         <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>94</v>
@@ -3169,10 +3169,10 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
         <v>31</v>
@@ -3187,66 +3187,66 @@
         <v>31</v>
       </c>
       <c r="J30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K30" t="s">
         <v>31</v>
       </c>
       <c r="L30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>96</v>
@@ -3255,10 +3255,10 @@
         <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
         <v>31</v>
@@ -3273,61 +3273,61 @@
         <v>31</v>
       </c>
       <c r="J31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K31" t="s">
         <v>31</v>
       </c>
       <c r="L31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32">
@@ -3341,84 +3341,84 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>101</v>
@@ -3427,84 +3427,84 @@
         <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I33" t="s">
         <v>31</v>
       </c>
       <c r="J33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
         <v>103</v>
@@ -3513,84 +3513,84 @@
         <v>104</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K34" t="s">
         <v>31</v>
       </c>
       <c r="L34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M34" t="s">
         <v>31</v>
       </c>
       <c r="N34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V34" t="s">
         <v>31</v>
       </c>
       <c r="W34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>105</v>
@@ -3599,79 +3599,79 @@
         <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F35" t="s">
         <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I35" t="s">
         <v>31</v>
       </c>
       <c r="J35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M35" t="s">
         <v>31</v>
       </c>
       <c r="N35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA35" t="s">
         <v>31</v>
       </c>
       <c r="AB35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>